<commit_message>
New message for the combined commit_
</commit_message>
<xml_diff>
--- a/data_analysis/PythonPipeline/PatientData/Patient9/Patient_9_SBS_Scores.xlsx
+++ b/data_analysis/PythonPipeline/PatientData/Patient9/Patient_9_SBS_Scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Desktop/DT/PedAccel/Data Analysis/FeatureExtraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b14a0d7b62cf6ad0/Sid Stuff/PROJECTS/iMEDS Design Team/Data Analysis/PedAccel/data_analysis/PythonPipeline/PatientData/Patient9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5461E38-4C18-B74B-A992-4EE46A3E2650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F5461E38-4C18-B74B-A992-4EE46A3E2650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E25476C-B4D3-4498-83A5-BABF50FBD05B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{809031ED-8969-471B-B3A5-4615F6501142}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{809031ED-8969-471B-B3A5-4615F6501142}"/>
   </bookViews>
   <sheets>
     <sheet name="SBS Scores" sheetId="1" r:id="rId1"/>
@@ -665,30 +665,30 @@
   <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="1" max="2" width="21.1328125" customWidth="1"/>
+    <col min="5" max="5" width="21.796875" customWidth="1"/>
     <col min="6" max="11" width="26" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -721,13 +721,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6" t="str">
-        <f>TEXT(A4,"M/dd/yyyy hh:mm::ss AM/PM")</f>
-        <v>1/15/2024  14:00:00 PM</v>
+      <c r="B4" s="6">
+        <f>E6</f>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -742,7 +742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -769,7 +769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -781,7 +781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -799,7 +799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -826,7 +826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -844,7 +844,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -910,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -925,7 +925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -943,7 +943,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
@@ -982,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
@@ -994,7 +994,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>35</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>36</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <v>45307</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <v>45307.041666666664</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <v>45307.083333333336</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <v>45307.109722222223</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <v>45307.116666666669</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
         <v>45307.125</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <v>45307.199305555558</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
         <v>45307.208333333336</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <v>45307.224999999999</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <v>45307.247916666667</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>0.49249999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="6">
         <v>45307.25</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="6">
         <v>45307.291666666664</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="6">
         <v>45307.333333333336</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="6">
         <v>45307.352083333331</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="6">
         <v>45307.375</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="6">
         <v>45307.390972222223</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="6">
         <v>45307.40625</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="6">
         <v>45307.416666666664</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="7">
         <v>45307.443055555559</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="7">
         <v>45307.458333333336</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
         <v>45307.484722222223</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="7">
         <v>45307.5</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="6" t="s">
         <v>40</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="6" t="s">
         <v>41</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="6" t="s">
         <v>42</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="6" t="s">
         <v>43</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="6" t="s">
         <v>44</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="6" t="s">
         <v>45</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="6" t="s">
         <v>46</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="6" t="s">
         <v>47</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="6" t="s">
         <v>49</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="6" t="s">
         <v>50</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="6" t="s">
         <v>51</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="6" t="s">
         <v>52</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="8">
         <v>45308</v>
       </c>
@@ -1672,7 +1672,7 @@
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="6">
         <v>45308.083333333336</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="6">
         <v>45308.152083333334</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="6">
         <v>45308.166666666664</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="6">
         <v>45308.18472222222</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="6">
         <v>45308.25</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="6">
         <v>45308.302777777775</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="6">
         <v>45308.30972222222</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="6">
         <v>45308.333333333336</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="6">
         <v>45308.395833333336</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="6">
         <v>45308.402777777781</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="6">
         <v>45308.459722222222</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="6">
         <v>45308.467361111114</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="6">
         <v>45308.5</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="6">
         <v>45308.538888888892</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="6" t="s">
         <v>54</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="6" t="s">
         <v>55</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="6" t="s">
         <v>56</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="6" t="s">
         <v>57</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="6" t="s">
         <v>58</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="6" t="s">
         <v>59</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="6" t="s">
         <v>60</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="6" t="s">
         <v>62</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="6" t="s">
         <v>63</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="6" t="s">
         <v>64</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="6" t="s">
         <v>65</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="6" t="s">
         <v>66</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="8">
         <v>45309</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="6">
         <v>45309.041666666664</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" s="6">
         <v>45309.097916666666</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="6">
         <v>45309.157638888886</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" s="6">
         <v>45309.166666666664</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A88" s="6">
         <v>45309.333333333336</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A89" s="6">
         <v>45309.350694444445</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A90" s="6">
         <v>45309.383333333331</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91" s="6">
         <v>45309.392361111109</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A92" s="6">
         <v>45309.416666666664</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A93" s="6">
         <v>45309.494444444441</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A94" s="6">
         <v>45309.5</v>
       </c>
@@ -2166,7 +2166,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>